<commit_message>
U001 - creating the menu-list component
</commit_message>
<xml_diff>
--- a/redchillidocs/DOCS/User-stories.xlsx
+++ b/redchillidocs/DOCS/User-stories.xlsx
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>PRIMARY REQUIREMENTS</t>
-  </si>
-  <si>
-    <t>Display red chilly menu items</t>
   </si>
   <si>
     <t xml:space="preserve">UI - add accordion(?) based list </t>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>Detect my location  deliver within ~3km</t>
+  </si>
+  <si>
+    <t>U001 - Display red chilly menu items</t>
   </si>
 </sst>
 </file>
@@ -432,15 +432,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,7 +737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -756,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="7">
         <v>43234</v>
@@ -851,56 +853,56 @@
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:23" s="5" customFormat="1">
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:23" s="5" customFormat="1">
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:23" s="5" customFormat="1">
       <c r="B7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:23" s="5" customFormat="1">
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:23" s="11" customFormat="1"/>
     <row r="10" spans="1:23" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:23" s="5" customFormat="1">
       <c r="B11" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:23" s="5" customFormat="1">
       <c r="B12" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="12"/>
     </row>
@@ -909,56 +911,56 @@
     </row>
     <row r="14" spans="1:23" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:23" s="5" customFormat="1">
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:23" s="5" customFormat="1">
       <c r="B16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" s="5" customFormat="1">
       <c r="B17" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1">
       <c r="B18" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" s="11" customFormat="1"/>
     <row r="20" spans="1:3" s="5" customFormat="1">
       <c r="A20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1">
       <c r="B21" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1">
-      <c r="B22" s="17" t="s">
-        <v>21</v>
+      <c r="B22" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -967,64 +969,64 @@
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1">
       <c r="A24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1">
       <c r="B25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" s="11" customFormat="1"/>
     <row r="27" spans="1:3" s="5" customFormat="1">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" s="5" customFormat="1" ht="60" customHeight="1">
+      <c r="A28" s="18"/>
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" s="5" customFormat="1">
+      <c r="A29" s="18"/>
+      <c r="B29" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" s="5" customFormat="1" ht="60" customHeight="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" s="5" customFormat="1">
-      <c r="A29" s="15"/>
-      <c r="B29" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1">
       <c r="B30" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1">
       <c r="B31" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1">
       <c r="B32" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" s="5" customFormat="1">
       <c r="B33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="6"/>
     </row>
@@ -1033,84 +1035,84 @@
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1">
       <c r="A35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3" s="5" customFormat="1">
       <c r="B36" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" s="5" customFormat="1">
       <c r="B37" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" s="5" customFormat="1">
       <c r="B38" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" s="5" customFormat="1">
       <c r="B39" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" s="11" customFormat="1"/>
     <row r="41" spans="1:3" s="5" customFormat="1">
       <c r="A41" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" s="5" customFormat="1">
       <c r="B42" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3" s="5" customFormat="1">
       <c r="B43" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" s="5" customFormat="1">
       <c r="B44" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1">
       <c r="B45" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" s="5" customFormat="1">
       <c r="B46" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" s="14" customFormat="1"/>
     <row r="48" spans="1:3" s="5" customFormat="1">
       <c r="A48" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="6"/>
     </row>
@@ -1125,61 +1127,61 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="14" customFormat="1"/>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="16" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="B58" s="16"/>
+      <c r="B58" s="19"/>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:23">
-      <c r="A66" s="18" t="s">
-        <v>66</v>
+      <c r="A66" s="16" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B68" s="4"/>
       <c r="D68" s="4"/>
@@ -1205,31 +1207,31 @@
     </row>
     <row r="69" spans="1:23">
       <c r="A69" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:23">
       <c r="A72" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:23">
       <c r="A73" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:23">
-      <c r="A75" s="19"/>
+      <c r="A75" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>